<commit_message>
Got the datasets uploaded into the python file
</commit_message>
<xml_diff>
--- a/Data/raw_data/Population/raw_pop_1600_1650.xlsx
+++ b/Data/raw_data/Population/raw_pop_1600_1650.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/954e9104582efe7e/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/954e9104582efe7e/Documents/Python/TEP4290_project/data/raw_data/Population/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF09E21B-C234-47DF-B5CC-AED508181686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{AF09E21B-C234-47DF-B5CC-AED508181686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CB2AEE6-C83E-403B-A802-191B7DB7AC74}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9F65BCBB-A17A-43B6-96E3-19020741FC59}"/>
   </bookViews>
@@ -36,9 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Population</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -393,12 +396,15 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>

</xml_diff>